<commit_message>
Command Line implementation added
</commit_message>
<xml_diff>
--- a/src/main/resources/FeatureConfiguration.xlsx
+++ b/src/main/resources/FeatureConfiguration.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772017FE-D8EF-417C-97EB-FCFEDCD2D558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB16567-C531-4A8D-8DB1-4219A6AFBCAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A31F56-4175-4006-83C8-54F694A7B0F3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5C3B48-D74F-497B-A84B-3ABD03A4135C}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>